<commit_message>
Fixed BOM errors, adjusted silkscreen labels
</commit_message>
<xml_diff>
--- a/resources/gbaHD-AIO-Shield.bom.xlsx
+++ b/resources/gbaHD-AIO-Shield.bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gameboy\Projects\gbaHD-AIO-Shield\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABC298F-BD49-4201-A2F9-A66D6AEF4D9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C521FE2B-9CDD-42A8-86E4-8DB44E315407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="765" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="146">
   <si>
     <t>Reference(s)</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Required</t>
   </si>
   <si>
-    <t>C1, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C16, C17, C21, C26</t>
-  </si>
-  <si>
     <t>0.1uF 0603</t>
   </si>
   <si>
@@ -88,15 +85,9 @@
     <t>100pF 0603</t>
   </si>
   <si>
-    <t>C15, C22, C27</t>
-  </si>
-  <si>
     <t>10uF 0805</t>
   </si>
   <si>
-    <t>D1, D4, D6</t>
-  </si>
-  <si>
     <t>Green LED 0603</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>Or generic, cut to size</t>
   </si>
   <si>
-    <t>D2, D3</t>
-  </si>
-  <si>
     <t>Schottky diode</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t>https://lcsc.com/product-detail/Schottky-Barrier-Diodes-SBD_Yangzhou-Yangjie-Elec-Tech-B5817WS_C699102.html</t>
   </si>
   <si>
-    <t>F1, F2, F3</t>
-  </si>
-  <si>
     <t>1.25A fuse 0603</t>
   </si>
   <si>
@@ -226,9 +211,6 @@
     <t>1uF 0603</t>
   </si>
   <si>
-    <t>C20</t>
-  </si>
-  <si>
     <t>Total 4 pieces including "Required" count</t>
   </si>
   <si>
@@ -437,6 +419,45 @@
   </si>
   <si>
     <t>Or use any switch of your choice</t>
+  </si>
+  <si>
+    <t>D1, D4</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>Or generic, total 3 pieces including "Required" count</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C1, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C16, C17, C21</t>
+  </si>
+  <si>
+    <t>Total 15 pieces including "Required" count</t>
+  </si>
+  <si>
+    <t>C15, C22</t>
+  </si>
+  <si>
+    <t>C20, C27</t>
+  </si>
+  <si>
+    <t>F1, F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Total 2 pieces including "Required" count</t>
+  </si>
+  <si>
+    <t>D3</t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -1332,7 +1353,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1438,13 +1459,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
-      </c>
-      <c r="C8">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -1458,13 +1479,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -1478,13 +1499,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>139</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -1498,53 +1519,53 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>29</v>
+        <v>145</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -1558,13 +1579,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1573,18 +1594,18 @@
         <v>7</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -1598,13 +1619,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -1618,13 +1639,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1638,13 +1659,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -1658,13 +1679,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -1678,13 +1699,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
@@ -1698,13 +1719,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>7</v>
@@ -1718,13 +1739,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -1744,13 +1765,13 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1761,13 +1782,13 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1778,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1795,13 +1816,13 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,13 +1833,13 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1829,33 +1850,33 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>7</v>
@@ -1863,19 +1884,19 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>7</v>
@@ -1883,443 +1904,523 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" t="s">
         <v>70</v>
       </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>19</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="F38" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>72</v>
       </c>
-      <c r="C33">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43">
         <v>2</v>
       </c>
-      <c r="D33" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" t="s">
-        <v>76</v>
-      </c>
-      <c r="F34" t="s">
-        <v>137</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" t="s">
-        <v>80</v>
-      </c>
-      <c r="F35" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="D43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
         <v>87</v>
       </c>
-      <c r="E37" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="G44" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>88</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
         <v>89</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="E45" t="s">
         <v>90</v>
       </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E39" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>92</v>
       </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
         <v>93</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="E46" t="s">
         <v>94</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E41" t="s">
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>96</v>
       </c>
-      <c r="F41" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="E47" t="s">
         <v>98</v>
       </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E42" t="s">
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>100</v>
       </c>
-      <c r="F42" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="3" t="s">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="E48" t="s">
         <v>102</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E43" t="s">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>104</v>
       </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="E49" t="s">
         <v>106</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E44" t="s">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F44" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="B51" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
         <v>110</v>
       </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F45" t="s">
-        <v>7</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
-        <v>116</v>
-      </c>
-      <c r="E47" t="s">
-        <v>7</v>
-      </c>
-      <c r="F47" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" t="s">
-        <v>117</v>
-      </c>
-      <c r="E48" t="s">
-        <v>118</v>
-      </c>
-      <c r="F48" t="s">
-        <v>28</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B50" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" t="s">
-        <v>122</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>123</v>
-      </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>124</v>
-      </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="F51" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>126</v>
+      <c r="G51" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>111</v>
+      </c>
+      <c r="E52" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>62</v>
+      </c>
+      <c r="E54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" t="s">
+        <v>119</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E57" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>125</v>
+      </c>
+      <c r="E58" t="s">
+        <v>126</v>
+      </c>
+      <c r="F58" t="s">
+        <v>132</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" t="s">
-        <v>128</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
-        <v>87</v>
-      </c>
-      <c r="E53" t="s">
-        <v>7</v>
-      </c>
-      <c r="F53" t="s">
-        <v>122</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>130</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54" t="s">
-        <v>131</v>
-      </c>
-      <c r="E54" t="s">
-        <v>132</v>
-      </c>
-      <c r="F54" t="s">
-        <v>138</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G54" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G51" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G48" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G45" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G44" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G43" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G42" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G41" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G36" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G35" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G58" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G55" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G52" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G49" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G48" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G47" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G46" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G39" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G38" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="G28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G27" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="G26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
@@ -2329,8 +2430,10 @@
     <hyperlink ref="G14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="G12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="G11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G36" r:id="rId21" xr:uid="{12A8EB8B-B10B-467E-A9B8-1C0B6F2D9C52}"/>
+    <hyperlink ref="G35" r:id="rId22" xr:uid="{C3966ED5-10A1-4D82-BC6C-2CBBE76A7939}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix BOM errors in spreadsheet
</commit_message>
<xml_diff>
--- a/resources/gbaHD-AIO-Shield.bom.xlsx
+++ b/resources/gbaHD-AIO-Shield.bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gameboy\Projects\gbaHD-AIO-Shield\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C521FE2B-9CDD-42A8-86E4-8DB44E315407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13A8850-E94E-4CA8-A17B-451124493325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="1" r:id="rId1"/>
@@ -1317,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,62 +1984,62 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>134</v>
+        <v>68</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="F36" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="F37" t="s">
-        <v>87</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>7</v>
+        <v>135</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="E38" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>71</v>
+        <v>87</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -2420,7 +2420,7 @@
     <hyperlink ref="G45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="G40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="G39" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G38" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G36" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="G28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G27" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="G26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
@@ -2430,8 +2430,8 @@
     <hyperlink ref="G14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="G12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
     <hyperlink ref="G11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G36" r:id="rId21" xr:uid="{12A8EB8B-B10B-467E-A9B8-1C0B6F2D9C52}"/>
-    <hyperlink ref="G35" r:id="rId22" xr:uid="{C3966ED5-10A1-4D82-BC6C-2CBBE76A7939}"/>
+    <hyperlink ref="G35" r:id="rId21" xr:uid="{C3966ED5-10A1-4D82-BC6C-2CBBE76A7939}"/>
+    <hyperlink ref="G37" r:id="rId22" xr:uid="{12A8EB8B-B10B-467E-A9B8-1C0B6F2D9C52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId23"/>

</xml_diff>